<commit_message>
Updated Tags for MAPD SNP Plan
Updated Tags for MAPD SNP Plan
</commit_message>
<xml_diff>
--- a/cukesatdd/src/main/resources/database/PlanDocs/DCE_MBD_MAPD_SNP_2022.xlsx
+++ b/cukesatdd/src/main/resources/database/PlanDocs/DCE_MBD_MAPD_SNP_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Hub Latest Project\mratdd\cukesatdd\src\main\resources\database\PlanDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89145573-D26B-4C87-907A-047A021EDA2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECB8685-128B-469E-8BBE-92E439CE00C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="30" windowWidth="19180" windowHeight="10170" tabRatio="670" activeTab="1" xr2:uid="{1C4A239E-242B-48E7-9378-A03FDEBEBF97}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="670" firstSheet="7" activeTab="10" xr2:uid="{1C4A239E-242B-48E7-9378-A03FDEBEBF97}"/>
   </bookViews>
   <sheets>
     <sheet name="MAPD_SNP_DCE" sheetId="1" r:id="rId1"/>
@@ -5471,7 +5471,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:Y461"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -40800,12 +40800,12 @@
   <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -40882,7 +40882,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>842</v>
       </c>
@@ -40959,7 +40959,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>844</v>
       </c>
@@ -41036,7 +41036,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>847</v>
       </c>
@@ -41113,7 +41113,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>850</v>
       </c>
@@ -41190,7 +41190,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>855</v>
       </c>
@@ -41267,7 +41267,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>860</v>
       </c>
@@ -41340,7 +41340,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>864</v>
       </c>
@@ -41413,7 +41413,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>871</v>
       </c>
@@ -41486,7 +41486,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>874</v>
       </c>
@@ -41559,7 +41559,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>878</v>
       </c>
@@ -41632,7 +41632,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>883</v>
       </c>
@@ -41705,7 +41705,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>886</v>
       </c>
@@ -41782,7 +41782,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>889</v>
       </c>
@@ -41859,7 +41859,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>891</v>
       </c>
@@ -41936,7 +41936,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>893</v>
       </c>
@@ -42013,7 +42013,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>897</v>
       </c>
@@ -42086,7 +42086,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>899</v>
       </c>
@@ -42159,7 +42159,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>904</v>
       </c>
@@ -42236,7 +42236,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>909</v>
       </c>
@@ -42313,7 +42313,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>912</v>
       </c>
@@ -42390,7 +42390,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>917</v>
       </c>
@@ -42463,7 +42463,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>920</v>
       </c>
@@ -42545,13 +42545,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2AB7959-320B-4FA3-A980-B7F66C2A47ED}">
   <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -42628,7 +42628,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>922</v>
       </c>
@@ -42701,7 +42701,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>926</v>
       </c>
@@ -42774,7 +42774,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>929</v>
       </c>
@@ -42851,7 +42851,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>931</v>
       </c>
@@ -42928,7 +42928,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>934</v>
       </c>
@@ -43001,7 +43001,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>938</v>
       </c>
@@ -43078,7 +43078,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>940</v>
       </c>
@@ -43155,7 +43155,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>942</v>
       </c>
@@ -43232,7 +43232,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>947</v>
       </c>
@@ -43305,7 +43305,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>949</v>
       </c>
@@ -43382,7 +43382,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>952</v>
       </c>
@@ -43459,7 +43459,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>954</v>
       </c>
@@ -43536,7 +43536,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>956</v>
       </c>
@@ -43613,7 +43613,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>958</v>
       </c>
@@ -43690,7 +43690,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>960</v>
       </c>
@@ -43767,7 +43767,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>963</v>
       </c>
@@ -43840,7 +43840,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>965</v>
       </c>
@@ -43913,7 +43913,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>967</v>
       </c>
@@ -43986,7 +43986,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>969</v>
       </c>
@@ -44059,7 +44059,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>975</v>
       </c>
@@ -44136,7 +44136,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>977</v>
       </c>
@@ -44213,7 +44213,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>979</v>
       </c>
@@ -58247,13 +58247,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D7B37F-B1BD-4AB3-B29A-B63AC58AAB9B}">
   <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -58330,7 +58330,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>98</v>
       </c>
@@ -58407,7 +58407,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>106</v>
       </c>
@@ -58484,7 +58484,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>111</v>
       </c>
@@ -58561,7 +58561,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>118</v>
       </c>
@@ -58638,7 +58638,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>123</v>
       </c>
@@ -58715,7 +58715,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>129</v>
       </c>
@@ -58792,7 +58792,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>136</v>
       </c>
@@ -58869,7 +58869,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>141</v>
       </c>
@@ -58946,7 +58946,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>143</v>
       </c>
@@ -59023,7 +59023,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>148</v>
       </c>
@@ -59100,7 +59100,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>150</v>
       </c>
@@ -59177,7 +59177,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>156</v>
       </c>
@@ -59254,7 +59254,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>164</v>
       </c>
@@ -59331,7 +59331,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>170</v>
       </c>
@@ -59408,7 +59408,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>177</v>
       </c>
@@ -59481,7 +59481,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>183</v>
       </c>
@@ -59554,7 +59554,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>190</v>
       </c>
@@ -59627,7 +59627,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>195</v>
       </c>
@@ -59700,7 +59700,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>199</v>
       </c>
@@ -59773,7 +59773,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>206</v>
       </c>
@@ -59846,7 +59846,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>212</v>
       </c>
@@ -59919,7 +59919,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>219</v>
       </c>
@@ -65068,12 +65068,12 @@
   <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -65150,7 +65150,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>225</v>
       </c>
@@ -65223,7 +65223,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>231</v>
       </c>
@@ -65296,7 +65296,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>235</v>
       </c>
@@ -65369,7 +65369,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>242</v>
       </c>
@@ -65442,7 +65442,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>247</v>
       </c>
@@ -65515,7 +65515,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>253</v>
       </c>
@@ -65588,7 +65588,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>259</v>
       </c>
@@ -65661,7 +65661,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>265</v>
       </c>
@@ -65734,7 +65734,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>269</v>
       </c>
@@ -65807,7 +65807,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>272</v>
       </c>
@@ -65880,7 +65880,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>276</v>
       </c>
@@ -65953,7 +65953,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>279</v>
       </c>
@@ -66026,7 +66026,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>285</v>
       </c>
@@ -66099,7 +66099,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>288</v>
       </c>
@@ -66172,7 +66172,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>291</v>
       </c>
@@ -66245,7 +66245,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>295</v>
       </c>
@@ -66318,7 +66318,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>298</v>
       </c>
@@ -66391,7 +66391,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>300</v>
       </c>
@@ -66464,7 +66464,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>302</v>
       </c>
@@ -66537,7 +66537,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>307</v>
       </c>
@@ -66610,7 +66610,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>309</v>
       </c>
@@ -66683,7 +66683,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>311</v>
       </c>
@@ -66766,12 +66766,12 @@
   <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+      <selection sqref="A1:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -66848,7 +66848,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>313</v>
       </c>
@@ -66921,7 +66921,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>318</v>
       </c>
@@ -66994,7 +66994,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>324</v>
       </c>
@@ -67067,7 +67067,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>330</v>
       </c>
@@ -67140,7 +67140,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>335</v>
       </c>
@@ -67213,7 +67213,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>341</v>
       </c>
@@ -67286,7 +67286,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>344</v>
       </c>
@@ -67359,7 +67359,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>350</v>
       </c>
@@ -67432,7 +67432,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>352</v>
       </c>
@@ -67505,7 +67505,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>356</v>
       </c>
@@ -67578,7 +67578,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>361</v>
       </c>
@@ -67651,7 +67651,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>363</v>
       </c>
@@ -67724,7 +67724,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>365</v>
       </c>
@@ -67797,7 +67797,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>367</v>
       </c>
@@ -67870,7 +67870,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>370</v>
       </c>
@@ -67943,7 +67943,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>373</v>
       </c>
@@ -68016,7 +68016,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>375</v>
       </c>
@@ -68089,7 +68089,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>377</v>
       </c>
@@ -68162,7 +68162,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>380</v>
       </c>
@@ -68235,7 +68235,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>382</v>
       </c>
@@ -68308,7 +68308,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>384</v>
       </c>
@@ -68381,7 +68381,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>386</v>
       </c>
@@ -68464,12 +68464,12 @@
   <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -68546,7 +68546,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>388</v>
       </c>
@@ -68619,7 +68619,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>394</v>
       </c>
@@ -68692,7 +68692,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>397</v>
       </c>
@@ -68765,7 +68765,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>399</v>
       </c>
@@ -68838,7 +68838,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>405</v>
       </c>
@@ -68911,7 +68911,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>407</v>
       </c>
@@ -68984,7 +68984,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>411</v>
       </c>
@@ -69057,7 +69057,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>416</v>
       </c>
@@ -69130,7 +69130,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>418</v>
       </c>
@@ -69203,7 +69203,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>424</v>
       </c>
@@ -69276,7 +69276,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>428</v>
       </c>
@@ -69349,7 +69349,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>431</v>
       </c>
@@ -69422,7 +69422,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>435</v>
       </c>
@@ -69495,7 +69495,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>440</v>
       </c>
@@ -69568,7 +69568,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>445</v>
       </c>
@@ -69641,7 +69641,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>447</v>
       </c>
@@ -69714,7 +69714,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>449</v>
       </c>
@@ -69787,7 +69787,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>452</v>
       </c>
@@ -69860,7 +69860,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>454</v>
       </c>
@@ -69933,7 +69933,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>456</v>
       </c>
@@ -70006,7 +70006,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>458</v>
       </c>
@@ -70079,7 +70079,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>462</v>
       </c>
@@ -70162,12 +70162,12 @@
   <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+      <selection sqref="A1:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -70244,7 +70244,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>464</v>
       </c>
@@ -70317,7 +70317,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>467</v>
       </c>
@@ -70390,7 +70390,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>469</v>
       </c>
@@ -70463,7 +70463,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>474</v>
       </c>
@@ -70536,7 +70536,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>478</v>
       </c>
@@ -70613,7 +70613,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>487</v>
       </c>
@@ -70690,7 +70690,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>500</v>
       </c>
@@ -70763,7 +70763,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>514</v>
       </c>
@@ -70836,7 +70836,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>522</v>
       </c>
@@ -70909,7 +70909,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>526</v>
       </c>
@@ -70986,7 +70986,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>528</v>
       </c>
@@ -71063,7 +71063,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>533</v>
       </c>
@@ -71140,7 +71140,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>537</v>
       </c>
@@ -71217,7 +71217,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>543</v>
       </c>
@@ -71294,7 +71294,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>548</v>
       </c>
@@ -71367,7 +71367,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>553</v>
       </c>
@@ -71444,7 +71444,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>558</v>
       </c>
@@ -71521,7 +71521,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>562</v>
       </c>
@@ -71598,7 +71598,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>566</v>
       </c>
@@ -71675,7 +71675,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>570</v>
       </c>
@@ -71752,7 +71752,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>575</v>
       </c>
@@ -71829,7 +71829,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>578</v>
       </c>
@@ -71916,12 +71916,12 @@
   <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -71998,7 +71998,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>580</v>
       </c>
@@ -72075,7 +72075,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>584</v>
       </c>
@@ -72148,7 +72148,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>590</v>
       </c>
@@ -72221,7 +72221,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>596</v>
       </c>
@@ -72294,7 +72294,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>599</v>
       </c>
@@ -72371,7 +72371,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>604</v>
       </c>
@@ -72448,7 +72448,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>608</v>
       </c>
@@ -72525,7 +72525,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>613</v>
       </c>
@@ -72602,7 +72602,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>618</v>
       </c>
@@ -72679,7 +72679,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>622</v>
       </c>
@@ -72756,7 +72756,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>626</v>
       </c>
@@ -72833,7 +72833,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>631</v>
       </c>
@@ -72910,7 +72910,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>633</v>
       </c>
@@ -72987,7 +72987,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>638</v>
       </c>
@@ -73060,7 +73060,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>643</v>
       </c>
@@ -73137,7 +73137,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>646</v>
       </c>
@@ -73214,7 +73214,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>650</v>
       </c>
@@ -73291,7 +73291,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>654</v>
       </c>
@@ -73368,7 +73368,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>659</v>
       </c>
@@ -73441,7 +73441,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>662</v>
       </c>
@@ -73514,7 +73514,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>665</v>
       </c>
@@ -73587,7 +73587,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>670</v>
       </c>
@@ -73670,12 +73670,12 @@
   <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -73752,7 +73752,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>674</v>
       </c>
@@ -73825,7 +73825,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>676</v>
       </c>
@@ -73898,7 +73898,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>680</v>
       </c>
@@ -73971,7 +73971,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>685</v>
       </c>
@@ -74044,7 +74044,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>691</v>
       </c>
@@ -74117,7 +74117,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>697</v>
       </c>
@@ -74190,7 +74190,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>701</v>
       </c>
@@ -74263,7 +74263,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>706</v>
       </c>
@@ -74336,7 +74336,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>710</v>
       </c>
@@ -74413,7 +74413,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>718</v>
       </c>
@@ -74490,7 +74490,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>721</v>
       </c>
@@ -74563,7 +74563,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>726</v>
       </c>
@@ -74636,7 +74636,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>730</v>
       </c>
@@ -74709,7 +74709,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>732</v>
       </c>
@@ -74782,7 +74782,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>735</v>
       </c>
@@ -74859,7 +74859,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>739</v>
       </c>
@@ -74936,7 +74936,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>742</v>
       </c>
@@ -75013,7 +75013,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>746</v>
       </c>
@@ -75090,7 +75090,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>748</v>
       </c>
@@ -75167,7 +75167,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>753</v>
       </c>
@@ -75244,7 +75244,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>758</v>
       </c>
@@ -75321,7 +75321,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>760</v>
       </c>
@@ -75408,12 +75408,12 @@
   <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -75490,7 +75490,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>763</v>
       </c>
@@ -75567,7 +75567,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>766</v>
       </c>
@@ -75644,7 +75644,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>770</v>
       </c>
@@ -75721,7 +75721,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>773</v>
       </c>
@@ -75798,7 +75798,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>775</v>
       </c>
@@ -75875,7 +75875,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>778</v>
       </c>
@@ -75952,7 +75952,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>780</v>
       </c>
@@ -76029,7 +76029,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>782</v>
       </c>
@@ -76106,7 +76106,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>788</v>
       </c>
@@ -76183,7 +76183,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>794</v>
       </c>
@@ -76260,7 +76260,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>797</v>
       </c>
@@ -76337,7 +76337,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>801</v>
       </c>
@@ -76414,7 +76414,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>803</v>
       </c>
@@ -76491,7 +76491,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>808</v>
       </c>
@@ -76568,7 +76568,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>810</v>
       </c>
@@ -76645,7 +76645,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>812</v>
       </c>
@@ -76718,7 +76718,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>818</v>
       </c>
@@ -76795,7 +76795,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>821</v>
       </c>
@@ -76872,7 +76872,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>824</v>
       </c>
@@ -76949,7 +76949,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>829</v>
       </c>
@@ -77026,7 +77026,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>834</v>
       </c>
@@ -77103,7 +77103,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>839</v>
       </c>

</xml_diff>

<commit_message>
Improved tags for plans
Improved tags for plans
</commit_message>
<xml_diff>
--- a/cukesatdd/src/main/resources/database/PlanDocs/DCE_MBD_MAPD_SNP_2022.xlsx
+++ b/cukesatdd/src/main/resources/database/PlanDocs/DCE_MBD_MAPD_SNP_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Hub Latest Project\mratdd\cukesatdd\src\main\resources\database\PlanDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECB8685-128B-469E-8BBE-92E439CE00C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41481E69-B7BA-4593-9608-D33BF77F296D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="670" firstSheet="7" activeTab="10" xr2:uid="{1C4A239E-242B-48E7-9378-A03FDEBEBF97}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="670" xr2:uid="{1C4A239E-242B-48E7-9378-A03FDEBEBF97}"/>
   </bookViews>
   <sheets>
     <sheet name="MAPD_SNP_DCE" sheetId="1" r:id="rId1"/>
@@ -5469,9 +5469,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB4716B9-5855-4A9D-A33D-E582871FB114}">
   <dimension ref="A1:Y497"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A461" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E467" sqref="E467"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -42545,7 +42545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2AB7959-320B-4FA3-A980-B7F66C2A47ED}">
   <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -44300,12 +44300,12 @@
   <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -44382,7 +44382,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>981</v>
       </c>
@@ -44459,7 +44459,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>983</v>
       </c>
@@ -44536,7 +44536,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>985</v>
       </c>
@@ -44613,7 +44613,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>987</v>
       </c>
@@ -44690,7 +44690,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>989</v>
       </c>
@@ -44767,7 +44767,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>991</v>
       </c>
@@ -44844,7 +44844,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>993</v>
       </c>
@@ -44921,7 +44921,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>995</v>
       </c>
@@ -44998,7 +44998,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>997</v>
       </c>
@@ -45075,7 +45075,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>999</v>
       </c>
@@ -45152,7 +45152,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>1001</v>
       </c>
@@ -45225,7 +45225,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>1003</v>
       </c>
@@ -45298,7 +45298,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>1005</v>
       </c>
@@ -45371,7 +45371,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>1007</v>
       </c>
@@ -45444,7 +45444,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>1009</v>
       </c>
@@ -45521,7 +45521,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>1014</v>
       </c>
@@ -45598,7 +45598,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>1018</v>
       </c>
@@ -45675,7 +45675,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>1022</v>
       </c>
@@ -45752,7 +45752,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>1027</v>
       </c>
@@ -45829,7 +45829,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>1032</v>
       </c>
@@ -45906,7 +45906,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>1036</v>
       </c>
@@ -45983,7 +45983,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>1040</v>
       </c>
@@ -46070,12 +46070,12 @@
   <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -46152,7 +46152,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1043</v>
       </c>
@@ -46229,7 +46229,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1048</v>
       </c>
@@ -46306,7 +46306,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1050</v>
       </c>
@@ -46379,7 +46379,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>1053</v>
       </c>
@@ -46452,7 +46452,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>1055</v>
       </c>
@@ -46529,7 +46529,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>1057</v>
       </c>
@@ -46606,7 +46606,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>1062</v>
       </c>
@@ -46683,7 +46683,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>1066</v>
       </c>
@@ -46760,7 +46760,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>1068</v>
       </c>
@@ -46833,7 +46833,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>1073</v>
       </c>
@@ -46906,7 +46906,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>1076</v>
       </c>
@@ -46979,7 +46979,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>1078</v>
       </c>
@@ -47056,7 +47056,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>1081</v>
       </c>
@@ -47133,7 +47133,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>1084</v>
       </c>
@@ -47210,7 +47210,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>1086</v>
       </c>
@@ -47287,7 +47287,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>1089</v>
       </c>
@@ -47364,7 +47364,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>1091</v>
       </c>
@@ -47441,7 +47441,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>1093</v>
       </c>
@@ -47518,7 +47518,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>1095</v>
       </c>
@@ -47595,7 +47595,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>1100</v>
       </c>
@@ -47672,7 +47672,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>1105</v>
       </c>
@@ -47745,7 +47745,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>1107</v>
       </c>
@@ -47828,12 +47828,12 @@
   <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -47910,7 +47910,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1113</v>
       </c>
@@ -47983,7 +47983,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1115</v>
       </c>
@@ -48056,7 +48056,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1117</v>
       </c>
@@ -48129,7 +48129,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>1122</v>
       </c>
@@ -48202,7 +48202,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>1125</v>
       </c>
@@ -48275,7 +48275,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>1130</v>
       </c>
@@ -48348,7 +48348,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>1132</v>
       </c>
@@ -48425,7 +48425,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>1134</v>
       </c>
@@ -48498,7 +48498,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>1136</v>
       </c>
@@ -48571,7 +48571,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>1138</v>
       </c>
@@ -48644,7 +48644,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>1140</v>
       </c>
@@ -48717,7 +48717,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>1147</v>
       </c>
@@ -48794,7 +48794,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>1151</v>
       </c>
@@ -48871,7 +48871,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>1153</v>
       </c>
@@ -48948,7 +48948,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>1158</v>
       </c>
@@ -49025,7 +49025,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>1161</v>
       </c>
@@ -49102,7 +49102,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>1165</v>
       </c>
@@ -49179,7 +49179,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>1167</v>
       </c>
@@ -49256,7 +49256,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>1171</v>
       </c>
@@ -49333,7 +49333,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>1173</v>
       </c>
@@ -49410,7 +49410,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>1179</v>
       </c>
@@ -49487,7 +49487,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>1182</v>
       </c>
@@ -49574,12 +49574,12 @@
   <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -49656,7 +49656,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1185</v>
       </c>
@@ -49733,7 +49733,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1187</v>
       </c>
@@ -49810,7 +49810,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1189</v>
       </c>
@@ -49887,7 +49887,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>1191</v>
       </c>
@@ -49964,7 +49964,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>1193</v>
       </c>
@@ -50037,7 +50037,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>1197</v>
       </c>
@@ -50110,7 +50110,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>1202</v>
       </c>
@@ -50183,7 +50183,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>1204</v>
       </c>
@@ -50256,7 +50256,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>1206</v>
       </c>
@@ -50329,7 +50329,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>1209</v>
       </c>
@@ -50402,7 +50402,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>1213</v>
       </c>
@@ -50475,7 +50475,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>1215</v>
       </c>
@@ -50548,7 +50548,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>1219</v>
       </c>
@@ -50621,7 +50621,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>1223</v>
       </c>
@@ -50694,7 +50694,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>1225</v>
       </c>
@@ -50767,7 +50767,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>1227</v>
       </c>
@@ -50840,7 +50840,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>1231</v>
       </c>
@@ -50913,7 +50913,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>1233</v>
       </c>
@@ -50986,7 +50986,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>1236</v>
       </c>
@@ -51059,7 +51059,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>1238</v>
       </c>
@@ -51132,7 +51132,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>1240</v>
       </c>
@@ -51205,7 +51205,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>1242</v>
       </c>
@@ -51288,12 +51288,12 @@
   <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -51370,7 +51370,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1246</v>
       </c>
@@ -51443,7 +51443,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1250</v>
       </c>
@@ -51516,7 +51516,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1255</v>
       </c>
@@ -51589,7 +51589,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>1258</v>
       </c>
@@ -51662,7 +51662,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>1260</v>
       </c>
@@ -51735,7 +51735,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>1262</v>
       </c>
@@ -51808,7 +51808,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>1264</v>
       </c>
@@ -51881,7 +51881,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>1269</v>
       </c>
@@ -51954,7 +51954,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>1271</v>
       </c>
@@ -52027,7 +52027,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>1273</v>
       </c>
@@ -52100,7 +52100,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>1275</v>
       </c>
@@ -52173,7 +52173,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>1277</v>
       </c>
@@ -52246,7 +52246,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>1279</v>
       </c>
@@ -52323,7 +52323,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>1282</v>
       </c>
@@ -52396,7 +52396,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>1284</v>
       </c>
@@ -52469,7 +52469,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>1287</v>
       </c>
@@ -52542,7 +52542,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>1289</v>
       </c>
@@ -52615,7 +52615,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>1291</v>
       </c>
@@ -52688,7 +52688,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>1295</v>
       </c>
@@ -52761,7 +52761,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>1297</v>
       </c>
@@ -52834,7 +52834,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>1299</v>
       </c>
@@ -52907,7 +52907,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>1302</v>
       </c>
@@ -52990,12 +52990,12 @@
   <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -53072,7 +53072,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1304</v>
       </c>
@@ -53145,7 +53145,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1306</v>
       </c>
@@ -53218,7 +53218,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1308</v>
       </c>
@@ -53291,7 +53291,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>1311</v>
       </c>
@@ -53364,7 +53364,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>1315</v>
       </c>
@@ -53437,7 +53437,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>1319</v>
       </c>
@@ -53510,7 +53510,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>1321</v>
       </c>
@@ -53583,7 +53583,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>1323</v>
       </c>
@@ -53656,7 +53656,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>1326</v>
       </c>
@@ -53729,7 +53729,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>1328</v>
       </c>
@@ -53802,7 +53802,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>1330</v>
       </c>
@@ -53875,7 +53875,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>1332</v>
       </c>
@@ -53948,7 +53948,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>1334</v>
       </c>
@@ -54021,7 +54021,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>1336</v>
       </c>
@@ -54094,7 +54094,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>1338</v>
       </c>
@@ -54167,7 +54167,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>1340</v>
       </c>
@@ -54240,7 +54240,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>1342</v>
       </c>
@@ -54313,7 +54313,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>1344</v>
       </c>
@@ -54386,7 +54386,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>1346</v>
       </c>
@@ -54463,7 +54463,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>1351</v>
       </c>
@@ -54540,7 +54540,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>1353</v>
       </c>
@@ -54617,7 +54617,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>1358</v>
       </c>
@@ -54704,12 +54704,12 @@
   <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -54786,7 +54786,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1361</v>
       </c>
@@ -54863,7 +54863,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1364</v>
       </c>
@@ -54936,7 +54936,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1369</v>
       </c>
@@ -55009,7 +55009,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>1371</v>
       </c>
@@ -55086,7 +55086,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>1373</v>
       </c>
@@ -55163,7 +55163,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>1375</v>
       </c>
@@ -55240,7 +55240,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>1380</v>
       </c>
@@ -55317,7 +55317,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>1382</v>
       </c>
@@ -55394,7 +55394,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>1384</v>
       </c>
@@ -55471,7 +55471,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>1387</v>
       </c>
@@ -55548,7 +55548,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>1391</v>
       </c>
@@ -55625,7 +55625,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>1393</v>
       </c>
@@ -55702,7 +55702,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>1396</v>
       </c>
@@ -55779,7 +55779,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>1400</v>
       </c>
@@ -55856,7 +55856,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>1403</v>
       </c>
@@ -55933,7 +55933,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>1408</v>
       </c>
@@ -56010,7 +56010,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>1410</v>
       </c>
@@ -56087,7 +56087,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>1412</v>
       </c>
@@ -56164,7 +56164,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>1415</v>
       </c>
@@ -56241,7 +56241,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>1418</v>
       </c>
@@ -56318,7 +56318,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>1421</v>
       </c>
@@ -56395,7 +56395,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>1423</v>
       </c>
@@ -56481,13 +56481,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CC6AC1A-C6DA-4FF9-868B-B02406D2BCF8}">
   <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -56564,7 +56564,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1425</v>
       </c>
@@ -56641,7 +56641,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1427</v>
       </c>
@@ -56718,7 +56718,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1429</v>
       </c>
@@ -56795,7 +56795,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>1431</v>
       </c>
@@ -56872,7 +56872,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>1433</v>
       </c>
@@ -56949,7 +56949,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>1435</v>
       </c>
@@ -57026,7 +57026,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>1438</v>
       </c>
@@ -57103,7 +57103,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>1442</v>
       </c>
@@ -57180,7 +57180,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>1444</v>
       </c>
@@ -57257,7 +57257,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>1446</v>
       </c>
@@ -57334,7 +57334,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>1448</v>
       </c>
@@ -57411,7 +57411,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>1451</v>
       </c>
@@ -57484,7 +57484,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>1453</v>
       </c>
@@ -57557,7 +57557,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>1455</v>
       </c>
@@ -57630,7 +57630,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>1457</v>
       </c>
@@ -57703,7 +57703,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>1459</v>
       </c>
@@ -57776,7 +57776,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>1461</v>
       </c>
@@ -57853,7 +57853,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>1463</v>
       </c>
@@ -57930,7 +57930,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>1465</v>
       </c>
@@ -58007,7 +58007,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>1467</v>
       </c>
@@ -58084,7 +58084,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>1469</v>
       </c>
@@ -58161,7 +58161,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>1471</v>
       </c>
@@ -60001,13 +60001,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{197AD6BB-7F35-488A-BC6C-7C77906A7356}">
   <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -60084,7 +60084,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1473</v>
       </c>
@@ -60161,7 +60161,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1476</v>
       </c>
@@ -60234,7 +60234,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1479</v>
       </c>
@@ -60307,7 +60307,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>1484</v>
       </c>
@@ -60382,7 +60382,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>1488</v>
       </c>
@@ -60455,7 +60455,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>1490</v>
       </c>
@@ -60528,7 +60528,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>1492</v>
       </c>
@@ -60605,7 +60605,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>1494</v>
       </c>
@@ -60682,7 +60682,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>1496</v>
       </c>
@@ -60759,7 +60759,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>1498</v>
       </c>
@@ -60832,7 +60832,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>1500</v>
       </c>
@@ -60905,7 +60905,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>1504</v>
       </c>
@@ -60978,7 +60978,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>1509</v>
       </c>
@@ -61051,7 +61051,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>1512</v>
       </c>
@@ -61124,7 +61124,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>1514</v>
       </c>
@@ -61197,7 +61197,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>1516</v>
       </c>
@@ -61270,7 +61270,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>1520</v>
       </c>
@@ -61343,7 +61343,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>1522</v>
       </c>
@@ -61416,7 +61416,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>1525</v>
       </c>
@@ -61489,7 +61489,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>1527</v>
       </c>
@@ -61562,7 +61562,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>1529</v>
       </c>
@@ -61635,7 +61635,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>1531</v>
       </c>
@@ -61717,13 +61717,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87B65936-C562-4CF6-9A71-3A9443AA2C30}">
   <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -61800,7 +61800,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1533</v>
       </c>
@@ -61877,7 +61877,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1535</v>
       </c>
@@ -61954,7 +61954,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1537</v>
       </c>
@@ -62031,7 +62031,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>1539</v>
       </c>
@@ -62108,7 +62108,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>1541</v>
       </c>
@@ -62181,7 +62181,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>1543</v>
       </c>
@@ -62254,7 +62254,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>1545</v>
       </c>
@@ -62331,7 +62331,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>1547</v>
       </c>
@@ -62408,7 +62408,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>1550</v>
       </c>
@@ -62485,7 +62485,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>1553</v>
       </c>
@@ -62562,7 +62562,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>1555</v>
       </c>
@@ -62639,7 +62639,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>1557</v>
       </c>
@@ -62716,7 +62716,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>1559</v>
       </c>
@@ -62793,7 +62793,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>1561</v>
       </c>
@@ -62870,7 +62870,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>1563</v>
       </c>
@@ -62943,7 +62943,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>1565</v>
       </c>
@@ -63016,7 +63016,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>1567</v>
       </c>
@@ -63093,7 +63093,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>1569</v>
       </c>
@@ -63166,7 +63166,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>1571</v>
       </c>
@@ -63239,7 +63239,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>1573</v>
       </c>
@@ -63312,7 +63312,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>1575</v>
       </c>
@@ -63389,7 +63389,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>1577</v>
       </c>
@@ -63471,13 +63471,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9A41781-0FFE-453E-8FAE-155EDD980CBF}">
   <dimension ref="A1:Y21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -63554,7 +63554,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1579</v>
       </c>
@@ -63627,7 +63627,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1581</v>
       </c>
@@ -63700,7 +63700,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1583</v>
       </c>
@@ -63773,7 +63773,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>1585</v>
       </c>
@@ -63850,7 +63850,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>1587</v>
       </c>
@@ -63927,7 +63927,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>1589</v>
       </c>
@@ -64000,7 +64000,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>1591</v>
       </c>
@@ -64077,7 +64077,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>1594</v>
       </c>
@@ -64154,7 +64154,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>1598</v>
       </c>
@@ -64231,7 +64231,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>1601</v>
       </c>
@@ -64308,7 +64308,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>1605</v>
       </c>
@@ -64381,7 +64381,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>1608</v>
       </c>
@@ -64454,7 +64454,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>1611</v>
       </c>
@@ -64527,7 +64527,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>1614</v>
       </c>
@@ -64604,7 +64604,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>1617</v>
       </c>
@@ -64681,7 +64681,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>1620</v>
       </c>
@@ -64758,7 +64758,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>1622</v>
       </c>
@@ -64835,7 +64835,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>1626</v>
       </c>
@@ -64908,7 +64908,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>1628</v>
       </c>
@@ -64981,7 +64981,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>1630</v>
       </c>

</xml_diff>